<commit_message>
arreglo FT de daños
</commit_message>
<xml_diff>
--- a/SuraClaims/EnviarValidar_Inspeccion.xlsx
+++ b/SuraClaims/EnviarValidar_Inspeccion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E92B279-9D6C-4211-A8B8-DAEF15A58F17}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F54DDC1-9FFA-42F5-A75A-B15A2504A644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AF74D057-6E01-4208-A115-80971374A007}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>ID</t>
   </si>
@@ -58,6 +58,15 @@
   </si>
   <si>
     <t>0420172008282</t>
+  </si>
+  <si>
+    <t>0420194406702</t>
+  </si>
+  <si>
+    <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>ssurgwsoadev4-oci.opc.oracleoutsourcing.com</t>
   </si>
 </sst>
 </file>
@@ -443,10 +452,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA01E7D-480B-457E-89FE-07C13B233011}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,14 +481,11 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -487,15 +493,36 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{3CF74974-29E3-462F-8B11-265F931C91B0}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{3CF74974-29E3-462F-8B11-265F931C91B0}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{E99A488F-CC35-4B53-932F-DC780AEF07E7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>